<commit_message>
Ensure latest version of Excel
</commit_message>
<xml_diff>
--- a/Codespace_Results.xlsx
+++ b/Codespace_Results.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="288" documentId="8_{D99E50AD-0983-4592-8B1A-9EEAF4AB5118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F83BAD46-DA2C-40B9-B277-42FCAE3057EA}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{261F18E4-BC6F-446B-AA29-FEFFED214DAD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{261F18E4-BC6F-446B-AA29-FEFFED214DAD}"/>
   </bookViews>
   <sheets>
     <sheet name="RSA" sheetId="1" r:id="rId1"/>
@@ -11951,10 +11951,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -12254,8 +12250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6B1155-50CF-4580-B701-1CB09A3CC347}">
   <dimension ref="A1:AN44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16013,7 +16009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E67957C-8B44-4A73-BA03-9C6A368A209C}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -17675,7 +17671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F9AE12-229B-42E7-BED9-7D4154EAAFA7}">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="Z50" sqref="Z50"/>
     </sheetView>
   </sheetViews>

</xml_diff>